<commit_message>
📜 docs: recipies ingredients, recipies tabs added
</commit_message>
<xml_diff>
--- a/recipies.xlsx
+++ b/recipies.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dthess/Documents/Sites/DSTCrockPotsCalcFE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA50CF51-BCDF-D244-B269-8E4EF26485C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C90CBA-D4D0-7F44-95E6-4DE20C9DBBC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{036ACE1D-E166-A541-B647-B8529897E253}"/>
+    <workbookView xWindow="33600" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{036ACE1D-E166-A541-B647-B8529897E253}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ingredients" sheetId="3" r:id="rId1"/>
+    <sheet name="recipies" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,6 +34,404 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="131">
+  <si>
+    <t>meats</t>
+  </si>
+  <si>
+    <t>Batilisk Wing</t>
+  </si>
+  <si>
+    <t>Drumstick</t>
+  </si>
+  <si>
+    <t>Eel</t>
+  </si>
+  <si>
+    <t>Fish</t>
+  </si>
+  <si>
+    <t>Frog Legs</t>
+  </si>
+  <si>
+    <t>Koalefant Trunk</t>
+  </si>
+  <si>
+    <t>Winter Koalefant Trunk</t>
+  </si>
+  <si>
+    <t>Leafy Meat</t>
+  </si>
+  <si>
+    <t>Meat</t>
+  </si>
+  <si>
+    <t>Monster Meat</t>
+  </si>
+  <si>
+    <t>Morsel</t>
+  </si>
+  <si>
+    <t>Guardian's Horn</t>
+  </si>
+  <si>
+    <t>Deerclops Eyeball</t>
+  </si>
+  <si>
+    <t>Cooked Eel</t>
+  </si>
+  <si>
+    <t>Cooked Fish</t>
+  </si>
+  <si>
+    <t>Cooked Frog Legs</t>
+  </si>
+  <si>
+    <t>Koalefant Trunk Steak</t>
+  </si>
+  <si>
+    <t>Cooked Leafy Meat</t>
+  </si>
+  <si>
+    <t>Cooked Meat</t>
+  </si>
+  <si>
+    <t>Cooked Monster Meat</t>
+  </si>
+  <si>
+    <t>Cooked Morsel</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>ing1</t>
+  </si>
+  <si>
+    <t>ing2</t>
+  </si>
+  <si>
+    <t>ing3</t>
+  </si>
+  <si>
+    <t>ing4</t>
+  </si>
+  <si>
+    <t>Ingredients</t>
+  </si>
+  <si>
+    <t>Effects</t>
+  </si>
+  <si>
+    <t>health</t>
+  </si>
+  <si>
+    <t>hunger</t>
+  </si>
+  <si>
+    <t>sanity</t>
+  </si>
+  <si>
+    <t>rot</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>ingredient</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>Fried Drumbstick</t>
+  </si>
+  <si>
+    <t>Jerky</t>
+  </si>
+  <si>
+    <t>Small Jerky</t>
+  </si>
+  <si>
+    <t>Cooked Batalisk Wing</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>Monster Food</t>
+  </si>
+  <si>
+    <t>Durian</t>
+  </si>
+  <si>
+    <t>Extra Smelly*</t>
+  </si>
+  <si>
+    <t>Mob Drops</t>
+  </si>
+  <si>
+    <t>Butter</t>
+  </si>
+  <si>
+    <t>Butterfly Wings</t>
+  </si>
+  <si>
+    <t>Egg</t>
+  </si>
+  <si>
+    <t>Cooked Egg</t>
+  </si>
+  <si>
+    <t>Honey</t>
+  </si>
+  <si>
+    <t>Phlegm</t>
+  </si>
+  <si>
+    <t>Tallbird Egg</t>
+  </si>
+  <si>
+    <t>Fried Tallbird Egg*</t>
+  </si>
+  <si>
+    <t>TallBird Egg Hatching*</t>
+  </si>
+  <si>
+    <t>Electric Milk</t>
+  </si>
+  <si>
+    <t>Glommer's Goop</t>
+  </si>
+  <si>
+    <t>Moon Moth Wings</t>
+  </si>
+  <si>
+    <t>Royal Jelly</t>
+  </si>
+  <si>
+    <t>Vegetables</t>
+  </si>
+  <si>
+    <t>Carrot</t>
+  </si>
+  <si>
+    <t>Corn</t>
+  </si>
+  <si>
+    <t>Pop Corn</t>
+  </si>
+  <si>
+    <t>Roasted Carrot*</t>
+  </si>
+  <si>
+    <t>Eggplant</t>
+  </si>
+  <si>
+    <t>Braised Eggplant*</t>
+  </si>
+  <si>
+    <t>Foliage</t>
+  </si>
+  <si>
+    <t>Glow Berry</t>
+  </si>
+  <si>
+    <t>Lichen</t>
+  </si>
+  <si>
+    <t>Mandrake</t>
+  </si>
+  <si>
+    <t>Cooked Mandrake</t>
+  </si>
+  <si>
+    <t>Pumpkin</t>
+  </si>
+  <si>
+    <t>Hot Pumpkin</t>
+  </si>
+  <si>
+    <t>Red Cap</t>
+  </si>
+  <si>
+    <t>Cooked Red Cap</t>
+  </si>
+  <si>
+    <t>Green Cap</t>
+  </si>
+  <si>
+    <t>Cooked Green Cap</t>
+  </si>
+  <si>
+    <t>Blue Cap</t>
+  </si>
+  <si>
+    <t>Cooked Blue Cap</t>
+  </si>
+  <si>
+    <t>Petals</t>
+  </si>
+  <si>
+    <t>Dark Petals*</t>
+  </si>
+  <si>
+    <t>Cactus Flesh</t>
+  </si>
+  <si>
+    <t>Cooked Cactus Flesh</t>
+  </si>
+  <si>
+    <t>Cactus Flower</t>
+  </si>
+  <si>
+    <t>Asparagus</t>
+  </si>
+  <si>
+    <t>Cooked Asparagus</t>
+  </si>
+  <si>
+    <t>Garlic</t>
+  </si>
+  <si>
+    <t>Roasted Garlic*</t>
+  </si>
+  <si>
+    <t>Kelp Fronds</t>
+  </si>
+  <si>
+    <t>Cooked Kelp Fronds</t>
+  </si>
+  <si>
+    <t>Dried Kelp Fronds*</t>
+  </si>
+  <si>
+    <t>Lesser Glow Berry</t>
+  </si>
+  <si>
+    <t>OnionRoasted Onion*</t>
+  </si>
+  <si>
+    <t>Pepper</t>
+  </si>
+  <si>
+    <t>Roasted Pepper*</t>
+  </si>
+  <si>
+    <t>Potato</t>
+  </si>
+  <si>
+    <t>Roasted Potato*</t>
+  </si>
+  <si>
+    <t>Ripe Stone Fruit</t>
+  </si>
+  <si>
+    <t>Cooked Ripe Stone Fruit</t>
+  </si>
+  <si>
+    <t>Succulent</t>
+  </si>
+  <si>
+    <t>Toma Root</t>
+  </si>
+  <si>
+    <t>Roasted Toma Root</t>
+  </si>
+  <si>
+    <t>Fruits</t>
+  </si>
+  <si>
+    <t>Barries</t>
+  </si>
+  <si>
+    <t>Roasted Berries*</t>
+  </si>
+  <si>
+    <t>Dragon Fruit</t>
+  </si>
+  <si>
+    <t>Prepared Dragon Fruit*</t>
+  </si>
+  <si>
+    <t>Extra Smelly Durian*</t>
+  </si>
+  <si>
+    <t>Pomegranate</t>
+  </si>
+  <si>
+    <t>Sliced Pomegranate*</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>Cooked Banana</t>
+  </si>
+  <si>
+    <t>Watermelon</t>
+  </si>
+  <si>
+    <t>Grilled Watermelon*</t>
+  </si>
+  <si>
+    <t>Juicy Berries</t>
+  </si>
+  <si>
+    <t>Roasted Juicy Berries*</t>
+  </si>
+  <si>
+    <t>Dairy</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Rot</t>
+  </si>
+  <si>
+    <t>Rotten Egg</t>
+  </si>
+  <si>
+    <t>Seeds</t>
+  </si>
+  <si>
+    <t>Toasted Seeds*</t>
+  </si>
+  <si>
+    <t>Crop Seeds</t>
+  </si>
+  <si>
+    <t>Birchnut</t>
+  </si>
+  <si>
+    <t>Roasted Birchnut*</t>
+  </si>
+  <si>
+    <t>Ice</t>
+  </si>
+  <si>
+    <t>Lune Tree Blossom</t>
+  </si>
+  <si>
+    <t>Twig</t>
+  </si>
+  <si>
+    <t>Inedibles</t>
+  </si>
+  <si>
+    <t>Bone Shards</t>
+  </si>
+  <si>
+    <t>Nightmare Fuel</t>
+  </si>
+  <si>
+    <t>Volt Goat Horn</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -66,8 +465,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,13 +783,710 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{424ED68C-D496-4342-81EE-3B53CD651D96}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A61271-92CA-3444-B094-6E5C25D34FB5}">
+  <dimension ref="A1:C118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B83" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B84" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B85" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B86" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>101</v>
+      </c>
+      <c r="B90" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B92" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B94" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B95" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B99" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B100" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B101" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B102" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>115</v>
+      </c>
+      <c r="B104" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B105" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>116</v>
+      </c>
+      <c r="B106" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B108" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B110" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B111" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B112" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B113" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>127</v>
+      </c>
+      <c r="B115" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B116" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B117" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B118" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E480F53-8A80-6F4D-9FE7-7866E8CFEE97}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>